<commit_message>
Updated cost data and shell scripts
</commit_message>
<xml_diff>
--- a/data/adaptation/options.xlsx
+++ b/data/adaptation/options.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioxfordnexus-my.sharepoint.com/personal/hert5230_ox_ac_uk/Documents/local/JEM/data/adaptation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F363B334-1C09-D246-BA7F-B7A019880165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{F363B334-1C09-D246-BA7F-B7A019880165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD3EA23D-75F5-B84C-BFFF-327B236149A2}"/>
   <bookViews>
-    <workbookView xWindow="3260" yWindow="2160" windowWidth="28040" windowHeight="17440" xr2:uid="{0BA75A22-2D34-CD48-AA1F-969013CB995D}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20620" xr2:uid="{0BA75A22-2D34-CD48-AA1F-969013CB995D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>option</t>
   </si>
   <si>
-    <t xml:space="preserve">Upgrade utility poles from wood to metal </t>
-  </si>
-  <si>
     <t>pole</t>
   </si>
   <si>
@@ -115,16 +113,54 @@
   </si>
   <si>
     <t xml:space="preserve">Add network redundancy </t>
+  </si>
+  <si>
+    <t>Substation flood protection</t>
+  </si>
+  <si>
+    <t>https://www.nationalgrid.com/uk/electricity-transmission/document/140911/download</t>
+  </si>
+  <si>
+    <t>Full protection from flooding</t>
+  </si>
+  <si>
+    <t>Based on National Grid analysis from the UK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upgrade utility poles from wood to steel </t>
+  </si>
+  <si>
+    <t>Cost data based on MISO Energy (U.S.)</t>
+  </si>
+  <si>
+    <t>https://cdn.misoenergy.org/20190212%20PSC%20Item%2005a%20Transmission%20Cost%20Estimation%20Guide%20for%20MTEP%202019_for%20review317692.pdf</t>
+  </si>
+  <si>
+    <t>$USD per substation</t>
+  </si>
+  <si>
+    <t>$USD/kV per asset</t>
+  </si>
+  <si>
+    <t>Results in a 76% reduction in damage index (Miyamoto 2019)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,13 +183,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -466,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAE36EB-5BA5-344A-A5BC-AB3E4F05E957}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="155" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,8 +516,11 @@
     <col min="1" max="1" width="43.1640625" customWidth="1"/>
     <col min="2" max="2" width="22.1640625" customWidth="1"/>
     <col min="3" max="3" width="19.83203125" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="39" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="75.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -486,45 +528,48 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
       <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
@@ -532,22 +577,22 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
         <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
@@ -555,85 +600,117 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
         <v>18</v>
       </c>
+      <c r="D9">
+        <v>4289168</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>26</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>800.19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H9" r:id="rId1" xr:uid="{E1E9DB70-8647-4248-BE19-921B0A416475}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>